<commit_message>
fixed some issues - still WIP - solution not solving the full puzzle yet
</commit_message>
<xml_diff>
--- a/resources/input.xlsx
+++ b/resources/input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokhvis\Work\code\experiments\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokhvis\Work\code\experiments\sudoku\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0866C67A-447E-4B04-9D77-1A7690FC7042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE07F04-B179-4649-9DDC-352B46031D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,20 +108,489 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="31">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,176 +871,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:10" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" ht="28.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="14">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="15">
         <v>8</v>
       </c>
-      <c r="H2">
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17">
         <v>1</v>
       </c>
-      <c r="J2">
+      <c r="I2" s="15"/>
+      <c r="J2" s="18">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="B3" s="19"/>
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="D3" s="7"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5">
         <v>8</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="20">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="21">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="C4" s="11"/>
+      <c r="D4" s="12">
         <v>6</v>
       </c>
-      <c r="G4">
+      <c r="E4" s="13"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="13">
         <v>2</v>
       </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="22"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" ht="28.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
+      <c r="B5" s="23"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="F5" s="9"/>
+      <c r="G5" s="10">
         <v>5</v>
       </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="24"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="20"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7">
+      <c r="B7" s="21"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13">
         <v>8</v>
       </c>
-      <c r="G7">
+      <c r="F7" s="11"/>
+      <c r="G7" s="12">
         <v>2</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="13">
         <v>9</v>
       </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10" ht="28.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8">
+      <c r="B8" s="25"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="8">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>6</v>
       </c>
-      <c r="H8">
+      <c r="F8" s="6"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="3">
         <v>4</v>
       </c>
-      <c r="J8">
+      <c r="I8" s="6"/>
+      <c r="J8" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="19">
         <v>2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>6</v>
       </c>
-      <c r="I9">
+      <c r="D9" s="7"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5">
         <v>9</v>
       </c>
+      <c r="J9" s="20"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="27">
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="C10" s="28"/>
+      <c r="D10" s="29">
         <v>4</v>
       </c>
-      <c r="I10">
+      <c r="E10" s="30"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="28">
         <v>7</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="31">
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="1:10" ht="28.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working stage 2 - started with stage 3
</commit_message>
<xml_diff>
--- a/resources/input.xlsx
+++ b/resources/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokhvis\Work\code\experiments\sudoku\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE07F04-B179-4649-9DDC-352B46031D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E688B6D4-0268-4A95-8335-9D0D794C9504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +95,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -496,100 +503,103 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -874,42 +884,42 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="1" customWidth="1"/>
     <col min="2" max="10" width="5.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" s="32" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="32" t="s">
         <v>8</v>
       </c>
     </row>
@@ -917,21 +927,21 @@
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="2">
         <v>9</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="3">
         <v>8</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17">
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5">
         <v>1</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="18">
+      <c r="I2" s="3"/>
+      <c r="J2" s="6">
         <v>7</v>
       </c>
     </row>
@@ -939,19 +949,19 @@
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="5">
+      <c r="B3" s="7"/>
+      <c r="C3" s="8">
         <v>1</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5">
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="8">
         <v>8</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="11">
         <v>6</v>
       </c>
     </row>
@@ -959,96 +969,96 @@
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="12">
         <v>4</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12">
+      <c r="C4" s="13"/>
+      <c r="D4" s="14">
         <v>6</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12">
+      <c r="E4" s="15"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14">
         <v>1</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="15">
         <v>2</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="22"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10" ht="28.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19">
         <v>1</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="20">
         <v>3</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10">
+      <c r="F5" s="18"/>
+      <c r="G5" s="19">
         <v>5</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="24"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="20"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15">
         <v>8</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12">
+      <c r="F7" s="13"/>
+      <c r="G7" s="14">
         <v>2</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="15">
         <v>9</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="22"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="16"/>
     </row>
     <row r="8" spans="1:10" ht="28.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="8">
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24">
         <v>5</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="25">
         <v>6</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="3">
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25">
         <v>4</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="23"/>
       <c r="J8" s="26">
         <v>1</v>
       </c>
@@ -1057,21 +1067,21 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="7">
         <v>2</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="8">
         <v>6</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5">
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="8">
         <v>9</v>
       </c>
-      <c r="J9" s="20"/>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -1099,6 +1109,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;9&amp;K000000 Information Classification: GENERAL</oddFooter>
   </headerFooter>

</xml_diff>